<commit_message>
Update Sskp excel reference
</commit_message>
<xml_diff>
--- a/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/sskp_vorlage.xlsx
+++ b/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/sskp_vorlage.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ws-intern\PlanPro-Git\eclipse-set\java\bundles\org.eclipse.set.feature\rootdir\data\export\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse\PlanPro\eclipse-set-snapshot-667\data\export\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC81FEC-5ED8-4B33-8300-45F0D9F22A5E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FBD6D3-B6AA-48D2-9AFE-AAA66BA890D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -159,11 +159,6 @@
 samkeit</t>
   </si>
   <si>
-    <t>PZB-
-Schutz-
-punkt</t>
-  </si>
-  <si>
     <t>Anfang</t>
   </si>
   <si>
@@ -192,22 +187,6 @@
   <si>
     <t>PZB-
 Schutzstrecke</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Abstand zu 
-Bezugs-element/
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>Zielsignal</t>
-    </r>
   </si>
   <si>
     <t>Abstand 
@@ -260,6 +239,15 @@
     <t>Energie-
 versorgung</t>
   </si>
+  <si>
+    <t>PZB-
+Schutzpunkt</t>
+  </si>
+  <si>
+    <t>Abstand zu 
+Bezugselement/
+Zielsignal</t>
+  </si>
 </sst>
 </file>
 
@@ -298,7 +286,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
@@ -743,7 +730,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -807,65 +794,12 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
@@ -915,22 +849,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -938,10 +856,59 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -953,15 +920,43 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1396,7 +1391,7 @@
   <dimension ref="A1:AP231"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3:R4"/>
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1404,11 +1399,11 @@
     <col min="1" max="1" width="4.140625" style="13" customWidth="1"/>
     <col min="2" max="2" width="6.85546875" style="14" customWidth="1"/>
     <col min="3" max="3" width="6.85546875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="9" style="8" customWidth="1"/>
+    <col min="5" max="5" width="8" style="6" customWidth="1"/>
     <col min="6" max="6" width="4.5703125" style="6" customWidth="1"/>
     <col min="7" max="7" width="4.5703125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="5.5703125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" style="6" customWidth="1"/>
     <col min="9" max="9" width="10.140625" style="6" customWidth="1"/>
     <col min="10" max="10" width="8.28515625" style="6" customWidth="1"/>
     <col min="11" max="11" width="5.85546875" style="7" customWidth="1"/>
@@ -1425,16 +1420,16 @@
     <col min="24" max="24" width="5.5703125" style="6" customWidth="1"/>
     <col min="25" max="25" width="8.140625" style="6" customWidth="1"/>
     <col min="26" max="26" width="7.42578125" style="6" customWidth="1"/>
-    <col min="27" max="27" width="27" style="14" customWidth="1"/>
+    <col min="27" max="27" width="24.140625" style="14" customWidth="1"/>
     <col min="28" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:42" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29"/>
+      <c r="A1" s="20"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1473,7 +1468,7 @@
       <c r="O1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="44" t="s">
+      <c r="P1" s="30" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="3" t="s">
@@ -1494,366 +1489,366 @@
       <c r="V1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="W1" s="43" t="s">
+      <c r="W1" s="29" t="s">
         <v>33</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Y1" s="45" t="s">
+      <c r="Y1" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="Z1" s="45" t="s">
+      <c r="Z1" s="31" t="s">
         <v>39</v>
       </c>
       <c r="AA1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB1" s="35"/>
+      <c r="AC1" s="35"/>
+      <c r="AD1" s="35"/>
+      <c r="AE1" s="35"/>
+      <c r="AF1" s="35"/>
+      <c r="AG1" s="35"/>
+      <c r="AH1" s="35"/>
+      <c r="AI1" s="35"/>
+      <c r="AJ1" s="35"/>
+      <c r="AK1" s="35"/>
+      <c r="AL1" s="35"/>
+      <c r="AM1" s="35"/>
+      <c r="AN1" s="35"/>
+      <c r="AO1" s="35"/>
+      <c r="AP1" s="35"/>
+    </row>
+    <row r="2" spans="1:42" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="33"/>
+      <c r="B2" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="48"/>
+      <c r="D2" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
+      <c r="V2" s="47"/>
+      <c r="W2" s="47"/>
+      <c r="X2" s="47"/>
+      <c r="Y2" s="47"/>
+      <c r="Z2" s="48"/>
+      <c r="AA2" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB2" s="35"/>
+      <c r="AC2" s="35"/>
+      <c r="AD2" s="35"/>
+      <c r="AE2" s="35"/>
+      <c r="AF2" s="35"/>
+      <c r="AG2" s="35"/>
+      <c r="AH2" s="35"/>
+      <c r="AI2" s="35"/>
+      <c r="AJ2" s="35"/>
+      <c r="AK2" s="35"/>
+      <c r="AL2" s="35"/>
+      <c r="AM2" s="35"/>
+      <c r="AN2" s="35"/>
+      <c r="AO2" s="35"/>
+      <c r="AP2" s="35"/>
+    </row>
+    <row r="3" spans="1:42" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="41"/>
+      <c r="B3" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="AB1" s="54"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="54"/>
-      <c r="AF1" s="54"/>
-      <c r="AG1" s="54"/>
-      <c r="AH1" s="54"/>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="54"/>
-      <c r="AL1" s="54"/>
-      <c r="AM1" s="54"/>
-      <c r="AN1" s="54"/>
-      <c r="AO1" s="54"/>
-      <c r="AP1" s="54"/>
-    </row>
-    <row r="2" spans="1:42" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="21"/>
-      <c r="AA2" s="46" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB2" s="54"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="54"/>
-      <c r="AF2" s="54"/>
-      <c r="AG2" s="54"/>
-      <c r="AH2" s="54"/>
-      <c r="AI2" s="54"/>
-      <c r="AJ2" s="54"/>
-      <c r="AK2" s="54"/>
-      <c r="AL2" s="54"/>
-      <c r="AM2" s="54"/>
-      <c r="AN2" s="54"/>
-      <c r="AO2" s="54"/>
-      <c r="AP2" s="54"/>
-    </row>
-    <row r="3" spans="1:42" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
-      <c r="B3" s="22" t="s">
+      <c r="C3" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="D3" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="23" t="s">
+      <c r="F3" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="62" t="s">
+      <c r="G3" s="56"/>
+      <c r="H3" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="23" t="s">
+      <c r="L3" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="K3" s="24" t="s">
+      <c r="M3" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="L3" s="60" t="s">
+      <c r="N3" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="M3" s="22" t="s">
+      <c r="O3" s="58"/>
+      <c r="P3" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="N3" s="26" t="s">
+      <c r="Q3" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="O3" s="27"/>
-      <c r="P3" s="58" t="s">
+      <c r="R3" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="Q3" s="34" t="s">
+      <c r="S3" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="T3" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="U3" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="R3" s="55" t="s">
+      <c r="V3" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="S3" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="T3" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="U3" s="23" t="s">
+      <c r="W3" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="V3" s="23" t="s">
+      <c r="X3" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y3" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z3" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="W3" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="X3" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y3" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z3" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="AA3" s="35"/>
-      <c r="AB3" s="54"/>
-      <c r="AC3" s="54"/>
-      <c r="AD3" s="54"/>
-      <c r="AE3" s="54"/>
-      <c r="AF3" s="54"/>
-      <c r="AG3" s="54"/>
-      <c r="AH3" s="54"/>
-      <c r="AI3" s="54"/>
-      <c r="AJ3" s="54"/>
-      <c r="AK3" s="54"/>
-      <c r="AL3" s="54"/>
-      <c r="AM3" s="54"/>
-      <c r="AN3" s="54"/>
-      <c r="AO3" s="54"/>
-      <c r="AP3" s="54"/>
+      <c r="AA3" s="36"/>
+      <c r="AB3" s="35"/>
+      <c r="AC3" s="35"/>
+      <c r="AD3" s="35"/>
+      <c r="AE3" s="35"/>
+      <c r="AF3" s="35"/>
+      <c r="AG3" s="35"/>
+      <c r="AH3" s="35"/>
+      <c r="AI3" s="35"/>
+      <c r="AJ3" s="35"/>
+      <c r="AK3" s="35"/>
+      <c r="AL3" s="35"/>
+      <c r="AM3" s="35"/>
+      <c r="AN3" s="35"/>
+      <c r="AO3" s="35"/>
+      <c r="AP3" s="35"/>
     </row>
     <row r="4" spans="1:42" s="2" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="48"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="31"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G4" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="30"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="61"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="33" t="s">
+      <c r="H4" s="45"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="O4" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="O4" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="P4" s="59"/>
-      <c r="Q4" s="57"/>
-      <c r="R4" s="56"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="31"/>
-      <c r="U4" s="31"/>
-      <c r="V4" s="31"/>
-      <c r="W4" s="31"/>
-      <c r="X4" s="31"/>
-      <c r="Y4" s="31"/>
-      <c r="Z4" s="32"/>
-      <c r="AA4" s="35"/>
-      <c r="AB4" s="54"/>
-      <c r="AC4" s="54"/>
-      <c r="AD4" s="54"/>
-      <c r="AE4" s="54"/>
-      <c r="AF4" s="54"/>
-      <c r="AG4" s="54"/>
-      <c r="AH4" s="54"/>
-      <c r="AI4" s="54"/>
-      <c r="AJ4" s="54"/>
-      <c r="AK4" s="54"/>
-      <c r="AL4" s="54"/>
-      <c r="AM4" s="54"/>
-      <c r="AN4" s="54"/>
-      <c r="AO4" s="54"/>
-      <c r="AP4" s="54"/>
+      <c r="P4" s="52"/>
+      <c r="Q4" s="50"/>
+      <c r="R4" s="54"/>
+      <c r="S4" s="45"/>
+      <c r="T4" s="38"/>
+      <c r="U4" s="38"/>
+      <c r="V4" s="38"/>
+      <c r="W4" s="38"/>
+      <c r="X4" s="38"/>
+      <c r="Y4" s="38"/>
+      <c r="Z4" s="40"/>
+      <c r="AA4" s="36"/>
+      <c r="AB4" s="35"/>
+      <c r="AC4" s="35"/>
+      <c r="AD4" s="35"/>
+      <c r="AE4" s="35"/>
+      <c r="AF4" s="35"/>
+      <c r="AG4" s="35"/>
+      <c r="AH4" s="35"/>
+      <c r="AI4" s="35"/>
+      <c r="AJ4" s="35"/>
+      <c r="AK4" s="35"/>
+      <c r="AL4" s="35"/>
+      <c r="AM4" s="35"/>
+      <c r="AN4" s="35"/>
+      <c r="AO4" s="35"/>
+      <c r="AP4" s="35"/>
     </row>
     <row r="5" spans="1:42" s="11" customFormat="1" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="47"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="37" t="s">
+      <c r="A5" s="33"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="38" t="s">
+      <c r="D5" s="22"/>
+      <c r="E5" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="39" t="s">
+      <c r="F5" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="G5" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39" t="s">
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="37" t="s">
+      <c r="K5" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="L5" s="39"/>
-      <c r="M5" s="40" t="s">
+      <c r="L5" s="25"/>
+      <c r="M5" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="39" t="s">
+      <c r="N5" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="39" t="s">
+      <c r="O5" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="P5" s="53" t="s">
+      <c r="P5" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="39" t="s">
+      <c r="Q5" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="R5" s="41"/>
-      <c r="S5" s="40" t="s">
+      <c r="R5" s="27"/>
+      <c r="S5" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="T5" s="39" t="s">
+      <c r="T5" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="U5" s="39" t="s">
+      <c r="U5" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="V5" s="39" t="s">
+      <c r="V5" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="W5" s="39"/>
-      <c r="X5" s="39"/>
-      <c r="Y5" s="39"/>
-      <c r="Z5" s="39"/>
-      <c r="AA5" s="42"/>
-      <c r="AB5" s="54"/>
-      <c r="AC5" s="54"/>
-      <c r="AD5" s="54"/>
-      <c r="AE5" s="54"/>
-      <c r="AF5" s="54"/>
-      <c r="AG5" s="54"/>
-      <c r="AH5" s="54"/>
-      <c r="AI5" s="54"/>
-      <c r="AJ5" s="54"/>
-      <c r="AK5" s="54"/>
-      <c r="AL5" s="54"/>
-      <c r="AM5" s="54"/>
-      <c r="AN5" s="54"/>
-      <c r="AO5" s="54"/>
-      <c r="AP5" s="54"/>
+      <c r="W5" s="25"/>
+      <c r="X5" s="25"/>
+      <c r="Y5" s="25"/>
+      <c r="Z5" s="25"/>
+      <c r="AA5" s="28"/>
+      <c r="AB5" s="35"/>
+      <c r="AC5" s="35"/>
+      <c r="AD5" s="35"/>
+      <c r="AE5" s="35"/>
+      <c r="AF5" s="35"/>
+      <c r="AG5" s="35"/>
+      <c r="AH5" s="35"/>
+      <c r="AI5" s="35"/>
+      <c r="AJ5" s="35"/>
+      <c r="AK5" s="35"/>
+      <c r="AL5" s="35"/>
+      <c r="AM5" s="35"/>
+      <c r="AN5" s="35"/>
+      <c r="AO5" s="35"/>
+      <c r="AP5" s="35"/>
     </row>
     <row r="6" spans="1:42" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="50"/>
-      <c r="M6" s="51"/>
-      <c r="N6" s="51"/>
-      <c r="O6" s="51"/>
-      <c r="P6" s="52"/>
-      <c r="Q6" s="51"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="51"/>
-      <c r="T6" s="51"/>
-      <c r="U6" s="17"/>
-      <c r="V6" s="51"/>
-      <c r="W6" s="17"/>
-      <c r="X6" s="17"/>
-      <c r="Y6" s="17"/>
-      <c r="Z6" s="17"/>
-      <c r="AA6" s="49"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="60"/>
+      <c r="O6" s="60"/>
+      <c r="P6" s="61"/>
+      <c r="Q6" s="60"/>
+      <c r="R6" s="35"/>
+      <c r="S6" s="60"/>
+      <c r="T6" s="60"/>
+      <c r="U6" s="35"/>
+      <c r="V6" s="60"/>
+      <c r="W6" s="35"/>
+      <c r="X6" s="35"/>
+      <c r="Y6" s="35"/>
+      <c r="Z6" s="35"/>
+      <c r="AA6" s="62"/>
     </row>
     <row r="7" spans="1:42" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="51"/>
-      <c r="N7" s="51"/>
-      <c r="O7" s="51"/>
-      <c r="P7" s="52"/>
-      <c r="Q7" s="51"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="51"/>
-      <c r="T7" s="51"/>
-      <c r="U7" s="17"/>
-      <c r="V7" s="51"/>
-      <c r="W7" s="17"/>
-      <c r="X7" s="17"/>
-      <c r="Y7" s="17"/>
-      <c r="Z7" s="17"/>
-      <c r="AA7" s="17"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="59"/>
+      <c r="M7" s="60"/>
+      <c r="N7" s="60"/>
+      <c r="O7" s="60"/>
+      <c r="P7" s="61"/>
+      <c r="Q7" s="60"/>
+      <c r="R7" s="35"/>
+      <c r="S7" s="60"/>
+      <c r="T7" s="60"/>
+      <c r="U7" s="35"/>
+      <c r="V7" s="60"/>
+      <c r="W7" s="35"/>
+      <c r="X7" s="35"/>
+      <c r="Y7" s="35"/>
+      <c r="Z7" s="35"/>
+      <c r="AA7" s="35"/>
     </row>
     <row r="8" spans="1:42" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17"/>
@@ -8353,6 +8348,22 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="L2:R2"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="S2:Z2"/>
+    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:U4"/>
     <mergeCell ref="AA3:AA4"/>
     <mergeCell ref="W3:W4"/>
     <mergeCell ref="Z3:Z4"/>
@@ -8367,22 +8378,6 @@
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="S2:Z2"/>
-    <mergeCell ref="X3:X4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="L2:R2"/>
-    <mergeCell ref="N3:O3"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.19685039370078741" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
@@ -8391,56 +8386,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E758A0F93049BE4CAD441F10C0D8186D" ma:contentTypeVersion="6" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="3d4e64bebabe581e87caa1b5e2dea503">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="576ce185-3b2e-4f75-8b7c-efeb82226bea" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="85eee936267896b8f15e0fd2c7a0c6ca" ns2:_="" ns3:_="">
     <xsd:import namespace="576ce185-3b2e-4f75-8b7c-efeb82226bea"/>
@@ -8652,13 +8606,54 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8679,22 +8674,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52AA9053-CA78-458B-BFEC-B0A103F9F68C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF743650-405A-4EB5-9BE5-79180E38FBC9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9CFCEAE-5A31-4E8D-871E-0FEB90E546B0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{044B22B7-1F1B-4A24-A516-CD5663BACD02}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8713,10 +8700,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9CFCEAE-5A31-4E8D-871E-0FEB90E546B0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF743650-405A-4EB5-9BE5-79180E38FBC9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52AA9053-CA78-458B-BFEC-B0A103F9F68C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update Sskp excel reference (#213)
* Update Sskp excel reference

* Update Sskp reference

* Update swtbot reference
</commit_message>
<xml_diff>
--- a/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/sskp_vorlage.xlsx
+++ b/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/sskp_vorlage.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ws-intern\PlanPro-Git\eclipse-set\java\bundles\org.eclipse.set.feature\rootdir\data\export\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse\eclipse\data\export\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC81FEC-5ED8-4B33-8300-45F0D9F22A5E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8706B50C-1D22-436F-91AF-DFC27A4EBD5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="10710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sskp_Beispielbefüllung" sheetId="15" r:id="rId1"/>
@@ -159,11 +159,6 @@
 samkeit</t>
   </si>
   <si>
-    <t>PZB-
-Schutz-
-punkt</t>
-  </si>
-  <si>
     <t>Anfang</t>
   </si>
   <si>
@@ -192,22 +187,6 @@
   <si>
     <t>PZB-
 Schutzstrecke</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Abstand zu 
-Bezugs-element/
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>Zielsignal</t>
-    </r>
   </si>
   <si>
     <t>Abstand 
@@ -260,6 +239,15 @@
     <t>Energie-
 versorgung</t>
   </si>
+  <si>
+    <t>PZB-
+Schutzpunkt</t>
+  </si>
+  <si>
+    <t>Abstand zu 
+Bezugselement/
+Zielsignal</t>
+  </si>
 </sst>
 </file>
 
@@ -298,7 +286,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
@@ -743,7 +730,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -807,65 +794,12 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
@@ -915,27 +849,71 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -944,14 +922,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -961,9 +954,11 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1395,8 +1390,8 @@
   </sheetPr>
   <dimension ref="A1:AP231"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3:R4"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1404,11 +1399,11 @@
     <col min="1" max="1" width="4.140625" style="13" customWidth="1"/>
     <col min="2" max="2" width="6.85546875" style="14" customWidth="1"/>
     <col min="3" max="3" width="6.85546875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="9" style="8" customWidth="1"/>
+    <col min="5" max="5" width="8" style="6" customWidth="1"/>
     <col min="6" max="6" width="4.5703125" style="6" customWidth="1"/>
     <col min="7" max="7" width="4.5703125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="5.5703125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" style="6" customWidth="1"/>
     <col min="9" max="9" width="10.140625" style="6" customWidth="1"/>
     <col min="10" max="10" width="8.28515625" style="6" customWidth="1"/>
     <col min="11" max="11" width="5.85546875" style="7" customWidth="1"/>
@@ -1425,16 +1420,16 @@
     <col min="24" max="24" width="5.5703125" style="6" customWidth="1"/>
     <col min="25" max="25" width="8.140625" style="6" customWidth="1"/>
     <col min="26" max="26" width="7.42578125" style="6" customWidth="1"/>
-    <col min="27" max="27" width="27" style="14" customWidth="1"/>
+    <col min="27" max="27" width="24.140625" style="14" customWidth="1"/>
     <col min="28" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:42" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29"/>
+      <c r="A1" s="20"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1473,7 +1468,7 @@
       <c r="O1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="44" t="s">
+      <c r="P1" s="30" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="3" t="s">
@@ -1494,366 +1489,366 @@
       <c r="V1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="W1" s="43" t="s">
+      <c r="W1" s="29" t="s">
         <v>33</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Y1" s="45" t="s">
+      <c r="Y1" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="Z1" s="45" t="s">
+      <c r="Z1" s="31" t="s">
         <v>39</v>
       </c>
       <c r="AA1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB1" s="35"/>
+      <c r="AC1" s="35"/>
+      <c r="AD1" s="35"/>
+      <c r="AE1" s="35"/>
+      <c r="AF1" s="35"/>
+      <c r="AG1" s="35"/>
+      <c r="AH1" s="35"/>
+      <c r="AI1" s="35"/>
+      <c r="AJ1" s="35"/>
+      <c r="AK1" s="35"/>
+      <c r="AL1" s="35"/>
+      <c r="AM1" s="35"/>
+      <c r="AN1" s="35"/>
+      <c r="AO1" s="35"/>
+      <c r="AP1" s="35"/>
+    </row>
+    <row r="2" spans="1:42" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="33"/>
+      <c r="B2" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="41"/>
+      <c r="D2" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" s="44"/>
+      <c r="U2" s="44"/>
+      <c r="V2" s="44"/>
+      <c r="W2" s="44"/>
+      <c r="X2" s="44"/>
+      <c r="Y2" s="44"/>
+      <c r="Z2" s="41"/>
+      <c r="AA2" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB2" s="35"/>
+      <c r="AC2" s="35"/>
+      <c r="AD2" s="35"/>
+      <c r="AE2" s="35"/>
+      <c r="AF2" s="35"/>
+      <c r="AG2" s="35"/>
+      <c r="AH2" s="35"/>
+      <c r="AI2" s="35"/>
+      <c r="AJ2" s="35"/>
+      <c r="AK2" s="35"/>
+      <c r="AL2" s="35"/>
+      <c r="AM2" s="35"/>
+      <c r="AN2" s="35"/>
+      <c r="AO2" s="35"/>
+      <c r="AP2" s="35"/>
+    </row>
+    <row r="3" spans="1:42" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="58"/>
+      <c r="B3" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="AB1" s="54"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="54"/>
-      <c r="AF1" s="54"/>
-      <c r="AG1" s="54"/>
-      <c r="AH1" s="54"/>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="54"/>
-      <c r="AL1" s="54"/>
-      <c r="AM1" s="54"/>
-      <c r="AN1" s="54"/>
-      <c r="AO1" s="54"/>
-      <c r="AP1" s="54"/>
-    </row>
-    <row r="2" spans="1:42" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="21"/>
-      <c r="AA2" s="46" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB2" s="54"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="54"/>
-      <c r="AF2" s="54"/>
-      <c r="AG2" s="54"/>
-      <c r="AH2" s="54"/>
-      <c r="AI2" s="54"/>
-      <c r="AJ2" s="54"/>
-      <c r="AK2" s="54"/>
-      <c r="AL2" s="54"/>
-      <c r="AM2" s="54"/>
-      <c r="AN2" s="54"/>
-      <c r="AO2" s="54"/>
-      <c r="AP2" s="54"/>
-    </row>
-    <row r="3" spans="1:42" s="2" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
-      <c r="B3" s="22" t="s">
+      <c r="C3" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="D3" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="23" t="s">
+      <c r="F3" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="62" t="s">
+      <c r="G3" s="46"/>
+      <c r="H3" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="59" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="23" t="s">
+      <c r="L3" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="K3" s="24" t="s">
+      <c r="M3" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="L3" s="60" t="s">
+      <c r="N3" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="M3" s="22" t="s">
+      <c r="O3" s="48"/>
+      <c r="P3" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="N3" s="26" t="s">
+      <c r="Q3" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="O3" s="27"/>
-      <c r="P3" s="58" t="s">
+      <c r="R3" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="Q3" s="34" t="s">
+      <c r="S3" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="T3" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="U3" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="R3" s="55" t="s">
+      <c r="V3" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="S3" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="T3" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="U3" s="23" t="s">
+      <c r="W3" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="V3" s="23" t="s">
+      <c r="X3" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y3" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z3" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="W3" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="X3" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y3" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z3" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="AA3" s="35"/>
-      <c r="AB3" s="54"/>
-      <c r="AC3" s="54"/>
-      <c r="AD3" s="54"/>
-      <c r="AE3" s="54"/>
-      <c r="AF3" s="54"/>
-      <c r="AG3" s="54"/>
-      <c r="AH3" s="54"/>
-      <c r="AI3" s="54"/>
-      <c r="AJ3" s="54"/>
-      <c r="AK3" s="54"/>
-      <c r="AL3" s="54"/>
-      <c r="AM3" s="54"/>
-      <c r="AN3" s="54"/>
-      <c r="AO3" s="54"/>
-      <c r="AP3" s="54"/>
+      <c r="AA3" s="55"/>
+      <c r="AB3" s="35"/>
+      <c r="AC3" s="35"/>
+      <c r="AD3" s="35"/>
+      <c r="AE3" s="35"/>
+      <c r="AF3" s="35"/>
+      <c r="AG3" s="35"/>
+      <c r="AH3" s="35"/>
+      <c r="AI3" s="35"/>
+      <c r="AJ3" s="35"/>
+      <c r="AK3" s="35"/>
+      <c r="AL3" s="35"/>
+      <c r="AM3" s="35"/>
+      <c r="AN3" s="35"/>
+      <c r="AO3" s="35"/>
+      <c r="AP3" s="35"/>
     </row>
     <row r="4" spans="1:42" s="2" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="48"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="31"/>
+      <c r="A4" s="58"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="50"/>
       <c r="F4" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G4" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="30"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="61"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="33" t="s">
+      <c r="H4" s="43"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="62"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="O4" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="O4" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="P4" s="59"/>
-      <c r="Q4" s="57"/>
-      <c r="R4" s="56"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="31"/>
-      <c r="U4" s="31"/>
-      <c r="V4" s="31"/>
-      <c r="W4" s="31"/>
-      <c r="X4" s="31"/>
-      <c r="Y4" s="31"/>
-      <c r="Z4" s="32"/>
-      <c r="AA4" s="35"/>
-      <c r="AB4" s="54"/>
-      <c r="AC4" s="54"/>
-      <c r="AD4" s="54"/>
-      <c r="AE4" s="54"/>
-      <c r="AF4" s="54"/>
-      <c r="AG4" s="54"/>
-      <c r="AH4" s="54"/>
-      <c r="AI4" s="54"/>
-      <c r="AJ4" s="54"/>
-      <c r="AK4" s="54"/>
-      <c r="AL4" s="54"/>
-      <c r="AM4" s="54"/>
-      <c r="AN4" s="54"/>
-      <c r="AO4" s="54"/>
-      <c r="AP4" s="54"/>
+      <c r="P4" s="64"/>
+      <c r="Q4" s="52"/>
+      <c r="R4" s="54"/>
+      <c r="S4" s="43"/>
+      <c r="T4" s="50"/>
+      <c r="U4" s="50"/>
+      <c r="V4" s="50"/>
+      <c r="W4" s="50"/>
+      <c r="X4" s="50"/>
+      <c r="Y4" s="50"/>
+      <c r="Z4" s="57"/>
+      <c r="AA4" s="55"/>
+      <c r="AB4" s="35"/>
+      <c r="AC4" s="35"/>
+      <c r="AD4" s="35"/>
+      <c r="AE4" s="35"/>
+      <c r="AF4" s="35"/>
+      <c r="AG4" s="35"/>
+      <c r="AH4" s="35"/>
+      <c r="AI4" s="35"/>
+      <c r="AJ4" s="35"/>
+      <c r="AK4" s="35"/>
+      <c r="AL4" s="35"/>
+      <c r="AM4" s="35"/>
+      <c r="AN4" s="35"/>
+      <c r="AO4" s="35"/>
+      <c r="AP4" s="35"/>
     </row>
     <row r="5" spans="1:42" s="11" customFormat="1" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="47"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="37" t="s">
+      <c r="A5" s="33"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="38" t="s">
+      <c r="D5" s="22"/>
+      <c r="E5" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="39" t="s">
+      <c r="F5" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="G5" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39" t="s">
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="37" t="s">
+      <c r="K5" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="L5" s="39"/>
-      <c r="M5" s="40" t="s">
+      <c r="L5" s="25"/>
+      <c r="M5" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="39" t="s">
+      <c r="N5" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="39" t="s">
+      <c r="O5" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="P5" s="53" t="s">
+      <c r="P5" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="39" t="s">
+      <c r="Q5" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="R5" s="41"/>
-      <c r="S5" s="40" t="s">
+      <c r="R5" s="27"/>
+      <c r="S5" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="T5" s="39" t="s">
+      <c r="T5" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="U5" s="39" t="s">
+      <c r="U5" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="V5" s="39" t="s">
+      <c r="V5" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="W5" s="39"/>
-      <c r="X5" s="39"/>
-      <c r="Y5" s="39"/>
-      <c r="Z5" s="39"/>
-      <c r="AA5" s="42"/>
-      <c r="AB5" s="54"/>
-      <c r="AC5" s="54"/>
-      <c r="AD5" s="54"/>
-      <c r="AE5" s="54"/>
-      <c r="AF5" s="54"/>
-      <c r="AG5" s="54"/>
-      <c r="AH5" s="54"/>
-      <c r="AI5" s="54"/>
-      <c r="AJ5" s="54"/>
-      <c r="AK5" s="54"/>
-      <c r="AL5" s="54"/>
-      <c r="AM5" s="54"/>
-      <c r="AN5" s="54"/>
-      <c r="AO5" s="54"/>
-      <c r="AP5" s="54"/>
+      <c r="W5" s="25"/>
+      <c r="X5" s="25"/>
+      <c r="Y5" s="25"/>
+      <c r="Z5" s="25"/>
+      <c r="AA5" s="28"/>
+      <c r="AB5" s="35"/>
+      <c r="AC5" s="35"/>
+      <c r="AD5" s="35"/>
+      <c r="AE5" s="35"/>
+      <c r="AF5" s="35"/>
+      <c r="AG5" s="35"/>
+      <c r="AH5" s="35"/>
+      <c r="AI5" s="35"/>
+      <c r="AJ5" s="35"/>
+      <c r="AK5" s="35"/>
+      <c r="AL5" s="35"/>
+      <c r="AM5" s="35"/>
+      <c r="AN5" s="35"/>
+      <c r="AO5" s="35"/>
+      <c r="AP5" s="35"/>
     </row>
     <row r="6" spans="1:42" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="50"/>
-      <c r="M6" s="51"/>
-      <c r="N6" s="51"/>
-      <c r="O6" s="51"/>
-      <c r="P6" s="52"/>
-      <c r="Q6" s="51"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="51"/>
-      <c r="T6" s="51"/>
-      <c r="U6" s="17"/>
-      <c r="V6" s="51"/>
-      <c r="W6" s="17"/>
-      <c r="X6" s="17"/>
-      <c r="Y6" s="17"/>
-      <c r="Z6" s="17"/>
-      <c r="AA6" s="49"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="35"/>
+      <c r="S6" s="37"/>
+      <c r="T6" s="37"/>
+      <c r="U6" s="35"/>
+      <c r="V6" s="37"/>
+      <c r="W6" s="35"/>
+      <c r="X6" s="35"/>
+      <c r="Y6" s="35"/>
+      <c r="Z6" s="35"/>
+      <c r="AA6" s="39"/>
     </row>
     <row r="7" spans="1:42" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="51"/>
-      <c r="N7" s="51"/>
-      <c r="O7" s="51"/>
-      <c r="P7" s="52"/>
-      <c r="Q7" s="51"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="51"/>
-      <c r="T7" s="51"/>
-      <c r="U7" s="17"/>
-      <c r="V7" s="51"/>
-      <c r="W7" s="17"/>
-      <c r="X7" s="17"/>
-      <c r="Y7" s="17"/>
-      <c r="Z7" s="17"/>
-      <c r="AA7" s="17"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="35"/>
+      <c r="S7" s="37"/>
+      <c r="T7" s="37"/>
+      <c r="U7" s="35"/>
+      <c r="V7" s="37"/>
+      <c r="W7" s="35"/>
+      <c r="X7" s="35"/>
+      <c r="Y7" s="35"/>
+      <c r="Z7" s="35"/>
+      <c r="AA7" s="35"/>
     </row>
     <row r="8" spans="1:42" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17"/>
@@ -8391,10 +8386,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_DCDateCreated xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <_dlc_DocId xmlns="576ce185-3b2e-4f75-8b7c-efeb82226bea">CS36PAW5EANU-7-19945</_dlc_DocId>
+    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <_dlc_DocIdUrl xmlns="576ce185-3b2e-4f75-8b7c-efeb82226bea">
+      <Url>https://vst.tu-dresden.de/planpro/_layouts/15/DocIdRedir.aspx?ID=CS36PAW5EANU-7-19945</Url>
+      <Description>CS36PAW5EANU-7-19945</Description>
+    </_dlc_DocIdUrl>
+    <_Revision xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <_DCDateModified xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <_Status xmlns="http://schemas.microsoft.com/sharepoint/v3/fields">Nicht begonnen</_Status>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -8440,7 +8452,7 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E758A0F93049BE4CAD441F10C0D8186D" ma:contentTypeVersion="6" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="3d4e64bebabe581e87caa1b5e2dea503">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="576ce185-3b2e-4f75-8b7c-efeb82226bea" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="85eee936267896b8f15e0fd2c7a0c6ca" ns2:_="" ns3:_="">
     <xsd:import namespace="576ce185-3b2e-4f75-8b7c-efeb82226bea"/>
@@ -8652,7 +8664,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -8661,24 +8673,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_DCDateCreated xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <_dlc_DocId xmlns="576ce185-3b2e-4f75-8b7c-efeb82226bea">CS36PAW5EANU-7-19945</_dlc_DocId>
-    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <_dlc_DocIdUrl xmlns="576ce185-3b2e-4f75-8b7c-efeb82226bea">
-      <Url>https://vst.tu-dresden.de/planpro/_layouts/15/DocIdRedir.aspx?ID=CS36PAW5EANU-7-19945</Url>
-      <Description>CS36PAW5EANU-7-19945</Description>
-    </_dlc_DocIdUrl>
-    <_Revision xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <_DCDateModified xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <_Status xmlns="http://schemas.microsoft.com/sharepoint/v3/fields">Nicht begonnen</_Status>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FBE6F5E-0FD6-4104-B02A-28BCFB30DE46}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="576ce185-3b2e-4f75-8b7c-efeb82226bea"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52AA9053-CA78-458B-BFEC-B0A103F9F68C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
@@ -8686,7 +8698,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9CFCEAE-5A31-4E8D-871E-0FEB90E546B0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
@@ -8694,7 +8706,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{044B22B7-1F1B-4A24-A516-CD5663BACD02}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8713,27 +8725,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF743650-405A-4EB5-9BE5-79180E38FBC9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FBE6F5E-0FD6-4104-B02A-28BCFB30DE46}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="576ce185-3b2e-4f75-8b7c-efeb82226bea"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>